<commit_message>
ajuste de la solicitud gráfica CN_06_02_CO
</commit_message>
<xml_diff>
--- a/fuentes/contenidos/grado06/guion02/SolicitudGrafica_CN_06_02_CO.xlsx
+++ b/fuentes/contenidos/grado06/guion02/SolicitudGrafica_CN_06_02_CO.xlsx
@@ -9,7 +9,7 @@
   <sheets>
     <sheet name="Solicitud de iconografía" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="144525" iterateCount="2" iterateDelta="10"/>
+  <calcPr calcId="144525"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="44">
   <si>
     <t>Asignatura:</t>
   </si>
@@ -97,9 +97,6 @@
     <t>Archivo Shutterstock o ruta en web</t>
   </si>
   <si>
-    <t>http://seresvivosliyi.blogspot.com/</t>
-  </si>
-  <si>
     <t>Ciencias Naturales</t>
   </si>
   <si>
@@ -115,24 +112,15 @@
     <t>Seres vivos</t>
   </si>
   <si>
-    <t>http://2.bp.blogspot.com/_Q1mZvSvjl2Q/S8t1SiT6BLI/AAAAAAAAAC0/ttpdrpdrC1k/s1600/celula-en-jpg.jpg</t>
-  </si>
-  <si>
     <t>Célula, partes y funciones</t>
   </si>
   <si>
-    <t xml:space="preserve">http://1.bp.blogspot.com/-y5vOSPClCLU/TZI31ko9MCI/AAAAAAAAAAQ/crtwzjFWv3Y/s320/celula-procariota-934178.jpeg </t>
-  </si>
-  <si>
     <t>Célula procariota</t>
   </si>
   <si>
     <t>Vertical</t>
   </si>
   <si>
-    <t>http://4.bp.blogspot.com/-_CE-TYV1NSI/Uaanoyc8V3I/AAAAAAAAC_A/Gsi5HX-8WJw/s1600/Celula.jpg</t>
-  </si>
-  <si>
     <t>Célula eucariota</t>
   </si>
   <si>
@@ -149,13 +137,59 @@
   </si>
   <si>
     <t>Marzo 25 de 2015</t>
+  </si>
+  <si>
+    <t> 76933603</t>
+  </si>
+  <si>
+    <t>Traducir los siguientes términos que se encuetran en ingles:
+Centrioles: centriolos
+Mitochondria: mitocondria
+Peroxisome: Peroxisoma
+Secretory vesicle: vesícula secretora
+Smooth endoplasmic reticulum: retículo endoplasmático liso
+Rough endoplasmic reticulum: retículo endoplasmático rugoso
+Lysosome: lisosoma
+Plasma membrane: membrana plasmática
+Golgi complex: aparato de Golgi
+Ribosomes: ribosomas</t>
+  </si>
+  <si>
+    <t>Traducir los siguientes términos que se encuentran en inglés:
+Flagellum: Flagelo
+Nucleoid (DNA): Nucleoide (ADN)
+Cell membrane: Membrana celular
+Cell wall: Pared celular
+Capsule: Cápsula
+Ribosome: Ribosoma
+Pilus: Pili</t>
+  </si>
+  <si>
+    <t> 112395593</t>
+  </si>
+  <si>
+    <t>Traducir los siguientes términos que se encuentran en ingles:
+Rough endoplasmic reticulum: retículo endoplasmático rugoso
+Smooth ER: Retículo endoplasmático liso
+Golgi apparatus: Aparato de Golgi
+Vesicles: Vesículas
+Microtubules: Microtúbulos
+Mitochondrion: Mitocondria
+Plasma membrane: Membrana plasmática
+Lysosome: Lisosoma
+Ribosomes: Ribosomas
+Microfilaments: Microfilamentos
+Centrioles: Centriolos
+Nuclear envelope: Membrana nuclear
+Nucleus: Núcleo
+Nuclear pore: Poro nuclear</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="13" x14ac:knownFonts="1">
+  <fonts count="14" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -166,11 +200,13 @@
     <font>
       <sz val="10"/>
       <name val="Century Gothic"/>
+      <family val="2"/>
     </font>
     <font>
       <b/>
       <sz val="10"/>
       <name val="Century Gothic"/>
+      <family val="2"/>
     </font>
     <font>
       <u/>
@@ -192,16 +228,19 @@
       <sz val="10"/>
       <color theme="1"/>
       <name val="Century Gothic"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Century Gothic"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="9"/>
       <color rgb="FF000000"/>
       <name val="Century Gothic"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="12"/>
@@ -231,6 +270,12 @@
       <color rgb="FF000000"/>
       <name val="Times New Roman"/>
       <family val="1"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color rgb="FF333333"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="6">
@@ -530,7 +575,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="52">
+  <cellStyleXfs count="51">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -582,9 +627,8 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="58">
+  <cellXfs count="59">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
@@ -676,6 +720,32 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -685,6 +755,9 @@
     <xf numFmtId="0" fontId="2" fillId="5" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -700,45 +773,17 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="51" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="51" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
   </cellXfs>
-  <cellStyles count="52">
+  <cellStyles count="51">
     <cellStyle name="Hipervínculo" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hipervínculo" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hipervínculo" xfId="5" builtinId="8" hidden="1"/>
@@ -764,7 +809,6 @@
     <cellStyle name="Hipervínculo" xfId="45" builtinId="8" hidden="1"/>
     <cellStyle name="Hipervínculo" xfId="47" builtinId="8" hidden="1"/>
     <cellStyle name="Hipervínculo" xfId="49" builtinId="8" hidden="1"/>
-    <cellStyle name="Hipervínculo" xfId="51" builtinId="8"/>
     <cellStyle name="Hipervínculo visitado" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Hipervínculo visitado" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Hipervínculo visitado" xfId="6" builtinId="9" hidden="1"/>
@@ -803,187 +847,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>8</xdr:col>
-      <xdr:colOff>349249</xdr:colOff>
-      <xdr:row>9</xdr:row>
-      <xdr:rowOff>31751</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>8</xdr:col>
-      <xdr:colOff>1882212</xdr:colOff>
-      <xdr:row>9</xdr:row>
-      <xdr:rowOff>1579564</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="2" name="1 Imagen"/>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1">
-          <a:extLst>
-            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
-            </a:ext>
-          </a:extLst>
-        </a:blip>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="13525499" y="1984376"/>
-          <a:ext cx="1532963" cy="1547813"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>8</xdr:col>
-      <xdr:colOff>306338</xdr:colOff>
-      <xdr:row>10</xdr:row>
-      <xdr:rowOff>79376</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>8</xdr:col>
-      <xdr:colOff>1959853</xdr:colOff>
-      <xdr:row>10</xdr:row>
-      <xdr:rowOff>1571625</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="3" name="2 Imagen"/>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2">
-          <a:extLst>
-            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
-            </a:ext>
-          </a:extLst>
-        </a:blip>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="13466713" y="3683001"/>
-          <a:ext cx="1653515" cy="1492249"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>8</xdr:col>
-      <xdr:colOff>648891</xdr:colOff>
-      <xdr:row>11</xdr:row>
-      <xdr:rowOff>111125</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>8</xdr:col>
-      <xdr:colOff>1762125</xdr:colOff>
-      <xdr:row>11</xdr:row>
-      <xdr:rowOff>1460500</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="4" name="3 Imagen"/>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3">
-          <a:extLst>
-            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
-            </a:ext>
-          </a:extLst>
-        </a:blip>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="13809266" y="5429250"/>
-          <a:ext cx="1113234" cy="1349375"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>8</xdr:col>
-      <xdr:colOff>285750</xdr:colOff>
-      <xdr:row>12</xdr:row>
-      <xdr:rowOff>114301</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>8</xdr:col>
-      <xdr:colOff>1946883</xdr:colOff>
-      <xdr:row>12</xdr:row>
-      <xdr:rowOff>1409701</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="5" name="4 Imagen"/>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId4">
-          <a:extLst>
-            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
-            </a:ext>
-          </a:extLst>
-        </a:blip>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="13506450" y="7029451"/>
-          <a:ext cx="1661133" cy="1295400"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1310,9 +1173,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N108"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="50" zoomScaleNormal="50" zoomScalePageLayoutView="140" workbookViewId="0">
-      <pane ySplit="9" topLeftCell="A11" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G16" sqref="G16"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="140" workbookViewId="0">
+      <pane ySplit="9" topLeftCell="A10" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.875" defaultRowHeight="13.5" x14ac:dyDescent="0.25"/>
@@ -1346,38 +1209,38 @@
       <c r="B2" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="46" t="s">
-        <v>26</v>
-      </c>
-      <c r="D2" s="40"/>
-      <c r="F2" s="41" t="s">
+      <c r="C2" s="50" t="s">
+        <v>25</v>
+      </c>
+      <c r="D2" s="51"/>
+      <c r="F2" s="52" t="s">
         <v>1</v>
       </c>
-      <c r="G2" s="42"/>
+      <c r="G2" s="53"/>
     </row>
     <row r="3" spans="1:14" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="1"/>
       <c r="B3" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="C3" s="43">
+      <c r="C3" s="54">
         <v>6</v>
       </c>
-      <c r="D3" s="44"/>
-      <c r="F3" s="57" t="s">
-        <v>42</v>
-      </c>
-      <c r="G3" s="45"/>
+      <c r="D3" s="55"/>
+      <c r="F3" s="56" t="s">
+        <v>38</v>
+      </c>
+      <c r="G3" s="57"/>
     </row>
     <row r="4" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A4" s="1"/>
       <c r="B4" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="C4" s="47" t="s">
-        <v>27</v>
-      </c>
-      <c r="D4" s="44"/>
+      <c r="C4" s="58" t="s">
+        <v>26</v>
+      </c>
+      <c r="D4" s="55"/>
       <c r="E4" s="5"/>
       <c r="F4" s="1"/>
       <c r="G4" s="1"/>
@@ -1389,10 +1252,10 @@
       <c r="B5" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="C5" s="49" t="s">
-        <v>29</v>
-      </c>
-      <c r="D5" s="37"/>
+      <c r="C5" s="46" t="s">
+        <v>28</v>
+      </c>
+      <c r="D5" s="47"/>
       <c r="E5" s="5"/>
       <c r="F5" s="1"/>
       <c r="G5" s="1"/>
@@ -1415,8 +1278,8 @@
       <c r="B7" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="C7" s="48" t="s">
-        <v>28</v>
+      <c r="C7" s="37" t="s">
+        <v>27</v>
       </c>
       <c r="F7" s="1"/>
       <c r="G7" s="1"/>
@@ -1429,10 +1292,10 @@
       <c r="C8" s="11"/>
       <c r="D8" s="11"/>
       <c r="E8" s="11"/>
-      <c r="F8" s="38" t="s">
+      <c r="F8" s="48" t="s">
         <v>14</v>
       </c>
-      <c r="G8" s="39"/>
+      <c r="G8" s="49"/>
       <c r="H8" s="18"/>
       <c r="I8" s="12"/>
       <c r="J8" s="2"/>
@@ -1474,8 +1337,8 @@
       <c r="A10" s="13" t="s">
         <v>17</v>
       </c>
-      <c r="B10" s="50" t="s">
-        <v>25</v>
+      <c r="B10" s="44" t="s">
+        <v>39</v>
       </c>
       <c r="C10" s="14" t="s">
         <v>9</v>
@@ -1484,7 +1347,7 @@
         <v>10</v>
       </c>
       <c r="E10" s="14" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="F10" s="14" t="str">
         <f>CONCATENATE($C$7,"_",A10,"_small")</f>
@@ -1494,17 +1357,17 @@
         <f>CONCATENATE($C$7,"_",A10,"_zoom")</f>
         <v>CN_06_02_CO_IMG01_zoom</v>
       </c>
-      <c r="H10" s="51" t="s">
-        <v>30</v>
+      <c r="H10" s="39" t="s">
+        <v>29</v>
       </c>
       <c r="I10" s="19"/>
     </row>
-    <row r="11" spans="1:14" s="12" customFormat="1" ht="135" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:14" s="12" customFormat="1" ht="261" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="13" t="s">
         <v>18</v>
       </c>
-      <c r="B11" s="53" t="s">
-        <v>31</v>
+      <c r="B11" s="43">
+        <v>142194109</v>
       </c>
       <c r="C11" s="14" t="s">
         <v>9</v>
@@ -1523,17 +1386,19 @@
         <f t="shared" ref="G11:G22" si="1">CONCATENATE($C$7,"_",A11,"_zoom")</f>
         <v>CN_06_02_CO_IMG02_zoom</v>
       </c>
-      <c r="H11" s="54" t="s">
-        <v>32</v>
-      </c>
-      <c r="I11" s="15"/>
-    </row>
-    <row r="12" spans="1:14" s="12" customFormat="1" ht="122.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H11" s="41" t="s">
+        <v>30</v>
+      </c>
+      <c r="I11" s="45" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="12" spans="1:14" s="12" customFormat="1" ht="158.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="13" t="s">
         <v>19</v>
       </c>
-      <c r="B12" s="55" t="s">
-        <v>33</v>
+      <c r="B12" s="43">
+        <v>145028542</v>
       </c>
       <c r="C12" s="14" t="s">
         <v>9</v>
@@ -1542,7 +1407,7 @@
         <v>10</v>
       </c>
       <c r="E12" s="14" t="s">
-        <v>35</v>
+        <v>11</v>
       </c>
       <c r="F12" s="14" t="str">
         <f t="shared" si="0"/>
@@ -1552,17 +1417,19 @@
         <f t="shared" si="1"/>
         <v>CN_06_02_CO_IMG03_zoom</v>
       </c>
-      <c r="H12" s="54" t="s">
-        <v>34</v>
-      </c>
-      <c r="I12" s="19"/>
-    </row>
-    <row r="13" spans="1:14" s="12" customFormat="1" ht="123.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H12" s="41" t="s">
+        <v>31</v>
+      </c>
+      <c r="I12" s="41" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="13" spans="1:14" s="12" customFormat="1" ht="283.5" x14ac:dyDescent="0.25">
       <c r="A13" s="13" t="s">
         <v>20</v>
       </c>
-      <c r="B13" s="53" t="s">
-        <v>36</v>
+      <c r="B13" s="44" t="s">
+        <v>42</v>
       </c>
       <c r="C13" s="14" t="s">
         <v>9</v>
@@ -1571,7 +1438,7 @@
         <v>10</v>
       </c>
       <c r="E13" s="14" t="s">
-        <v>11</v>
+        <v>32</v>
       </c>
       <c r="F13" s="14" t="str">
         <f t="shared" si="0"/>
@@ -1581,17 +1448,19 @@
         <f t="shared" si="1"/>
         <v>CN_06_02_CO_IMG04_zoom</v>
       </c>
-      <c r="H13" s="54" t="s">
-        <v>37</v>
-      </c>
-      <c r="I13" s="19"/>
+      <c r="H13" s="41" t="s">
+        <v>33</v>
+      </c>
+      <c r="I13" s="41" t="s">
+        <v>43</v>
+      </c>
     </row>
     <row r="14" spans="1:14" s="12" customFormat="1" ht="94.5" x14ac:dyDescent="0.25">
       <c r="A14" s="13" t="s">
         <v>21</v>
       </c>
-      <c r="B14" s="50" t="s">
-        <v>38</v>
+      <c r="B14" s="38" t="s">
+        <v>34</v>
       </c>
       <c r="C14" s="14" t="s">
         <v>9</v>
@@ -1610,8 +1479,8 @@
         <f t="shared" si="1"/>
         <v>CN_06_02_CO_IMG05_zoom</v>
       </c>
-      <c r="H14" s="50" t="s">
-        <v>39</v>
+      <c r="H14" s="38" t="s">
+        <v>35</v>
       </c>
       <c r="I14" s="19"/>
     </row>
@@ -1619,8 +1488,8 @@
       <c r="A15" s="13" t="s">
         <v>22</v>
       </c>
-      <c r="B15" s="52" t="s">
-        <v>40</v>
+      <c r="B15" s="40" t="s">
+        <v>36</v>
       </c>
       <c r="C15" s="14" t="s">
         <v>9</v>
@@ -1628,8 +1497,8 @@
       <c r="D15" s="14" t="s">
         <v>10</v>
       </c>
-      <c r="E15" s="51" t="s">
-        <v>35</v>
+      <c r="E15" s="39" t="s">
+        <v>32</v>
       </c>
       <c r="F15" s="14" t="str">
         <f t="shared" si="0"/>
@@ -1639,8 +1508,8 @@
         <f t="shared" si="1"/>
         <v>CN_06_02_CO_IMG06_zoom</v>
       </c>
-      <c r="H15" s="56" t="s">
-        <v>41</v>
+      <c r="H15" s="42" t="s">
+        <v>37</v>
       </c>
       <c r="I15" s="21"/>
     </row>
@@ -2730,14 +2599,8 @@
       <formula1>"Ilustración,Fotografía"</formula1>
     </dataValidation>
   </dataValidations>
-  <hyperlinks>
-    <hyperlink ref="B11" r:id="rId1"/>
-    <hyperlink ref="B12" r:id="rId2" display="http://1.bp.blogspot.com/-y5vOSPClCLU/TZI31ko9MCI/AAAAAAAAAAQ/crtwzjFWv3Y/s320/celula-procariota-934178.jpeg"/>
-    <hyperlink ref="B13" r:id="rId3"/>
-  </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292" r:id="rId4"/>
-  <drawing r:id="rId5"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292" r:id="rId1"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>

</xml_diff>